<commit_message>
ternary plots and failed stacked bar plot experiments
</commit_message>
<xml_diff>
--- a/Marta/Egypt/Egypt.xlsx
+++ b/Marta/Egypt/Egypt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\MB\Marta\Egypt exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\MB\Marta\Egypt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -247,6 +250,2547 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Clay</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>B006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>B286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>B242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>B009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>B012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>B264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>B013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>B287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>B014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>B244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>B226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>B232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>B273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>B003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>B272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>B011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>B004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>B010</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>B007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>B002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>B008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>B005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>10.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>51.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50.31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60.45</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-18AA-413C-8160-0CB8E60DFE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Silt </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>B006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>B286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>B242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>B009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>B012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>B264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>B013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>B287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>B014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>B244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>B226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>B232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>B273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>B003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>B272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>B011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>B004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>B010</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>B007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>B002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>B008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>B005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>26.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.07</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37.33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.47</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.51</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.51</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17.45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-18AA-413C-8160-0CB8E60DFE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sand </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>B006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>B286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>B242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>B009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>B012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>B264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>B013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>B287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>B014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>B244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>B226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>B232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>B273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>B003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>B272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>B011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>B004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>B010</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>B007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>B002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>B008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>B005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.78</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34.71</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32.49</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28.55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-18AA-413C-8160-0CB8E60DFE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="559060616"/>
+        <c:axId val="559065536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="559060616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="559065536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="559065536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="559060616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fine </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>B006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>B286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>B242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>B009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>B012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>B264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>B013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>B287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>B014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>B244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>B226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>B232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>B273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>B003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>B272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>B011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>B004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>B010</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>B007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>B002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>B008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>B005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.63</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47.68</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>54.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60.74</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>67.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>67.77</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>71.45</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>72.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F41-43FA-9194-CB644D3BA8E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coarse </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>B006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>B286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>B242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>B009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>B012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>B264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>B013</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>B287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>B014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>B244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>B226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>B232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>B273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>B003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>B272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>B011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>B004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>B010</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>B007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>B002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>B008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>B005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.78</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34.71</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32.49</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28.55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1F41-43FA-9194-CB644D3BA8E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="556125824"/>
+        <c:axId val="556120904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="556125824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556120904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="556120904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556125824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>412749</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>110489</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,7 +3059,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +3105,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -573,19 +3117,19 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>24.48</v>
+        <v>10.59</v>
       </c>
       <c r="F2">
-        <v>15.07</v>
+        <v>26.51</v>
       </c>
       <c r="G2">
-        <v>60.46</v>
+        <v>62.9</v>
       </c>
       <c r="H2">
-        <v>39.54</v>
+        <v>37.1</v>
       </c>
       <c r="I2">
-        <v>60.46</v>
+        <v>62.9</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -593,63 +3137,63 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3">
-        <v>50.31</v>
+        <v>10.65</v>
       </c>
       <c r="F3">
-        <v>17.45</v>
+        <v>27.27</v>
       </c>
       <c r="G3">
-        <v>32.229999999999997</v>
+        <v>62.07</v>
       </c>
       <c r="H3">
-        <v>67.77</v>
+        <v>37.93</v>
       </c>
       <c r="I3">
-        <v>32.229999999999997</v>
+        <v>62.07</v>
       </c>
       <c r="J3">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>40.1</v>
+        <v>22.6</v>
       </c>
       <c r="F4">
-        <v>10.11</v>
+        <v>16.62</v>
       </c>
       <c r="G4">
-        <v>49.78</v>
+        <v>60.78</v>
       </c>
       <c r="H4">
-        <v>50.22</v>
+        <v>39.22</v>
       </c>
       <c r="I4">
-        <v>49.78</v>
+        <v>60.78</v>
       </c>
       <c r="J4">
         <v>20</v>
@@ -657,223 +3201,223 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>51.6</v>
+        <v>24.48</v>
       </c>
       <c r="F5">
-        <v>11.04</v>
+        <v>15.07</v>
       </c>
       <c r="G5">
-        <v>37.369999999999997</v>
+        <v>60.46</v>
       </c>
       <c r="H5">
-        <v>62.63</v>
+        <v>39.54</v>
       </c>
       <c r="I5">
-        <v>37.369999999999997</v>
+        <v>60.46</v>
       </c>
       <c r="J5">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>59.17</v>
+        <v>15.48</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>25.96</v>
       </c>
       <c r="G6">
-        <v>27.83</v>
+        <v>58.56</v>
       </c>
       <c r="H6">
-        <v>72.17</v>
+        <v>41.44</v>
       </c>
       <c r="I6">
-        <v>27.83</v>
+        <v>58.56</v>
       </c>
       <c r="J6">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7">
-        <v>10.59</v>
+        <v>10.91</v>
       </c>
       <c r="F7">
-        <v>26.51</v>
+        <v>30.58</v>
       </c>
       <c r="G7">
-        <v>62.9</v>
+        <v>58.51</v>
       </c>
       <c r="H7">
-        <v>37.1</v>
+        <v>41.49</v>
       </c>
       <c r="I7">
-        <v>62.9</v>
+        <v>58.51</v>
       </c>
       <c r="J7">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8">
-        <v>58</v>
+        <v>30.2</v>
       </c>
       <c r="F8">
-        <v>9.51</v>
+        <v>12.59</v>
       </c>
       <c r="G8">
-        <v>32.49</v>
+        <v>57.2</v>
       </c>
       <c r="H8">
-        <v>67.510000000000005</v>
+        <v>42.8</v>
       </c>
       <c r="I8">
-        <v>32.49</v>
+        <v>57.2</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9">
-        <v>60.45</v>
+        <v>21.66</v>
       </c>
       <c r="F9">
-        <v>10.99</v>
+        <v>21.76</v>
       </c>
       <c r="G9">
-        <v>28.55</v>
+        <v>56.59</v>
       </c>
       <c r="H9">
-        <v>71.45</v>
+        <v>43.41</v>
       </c>
       <c r="I9">
-        <v>28.55</v>
+        <v>56.59</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10">
-        <v>10.91</v>
+        <v>27.25</v>
       </c>
       <c r="F10">
-        <v>30.58</v>
+        <v>16.78</v>
       </c>
       <c r="G10">
-        <v>58.51</v>
+        <v>55.97</v>
       </c>
       <c r="H10">
-        <v>41.49</v>
+        <v>44.03</v>
       </c>
       <c r="I10">
-        <v>58.51</v>
+        <v>55.97</v>
       </c>
       <c r="J10">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>54.11</v>
+        <v>6.88</v>
       </c>
       <c r="F11">
-        <v>11.18</v>
+        <v>37.33</v>
       </c>
       <c r="G11">
-        <v>34.71</v>
+        <v>55.8</v>
       </c>
       <c r="H11">
-        <v>65.290000000000006</v>
+        <v>44.2</v>
       </c>
       <c r="I11">
-        <v>34.71</v>
+        <v>55.8</v>
       </c>
       <c r="J11">
         <v>20</v>
@@ -881,7 +3425,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>55</v>
@@ -893,19 +3437,19 @@
         <v>13</v>
       </c>
       <c r="E12">
-        <v>32.229999999999997</v>
+        <v>21.01</v>
       </c>
       <c r="F12">
-        <v>28.51</v>
+        <v>25.2</v>
       </c>
       <c r="G12">
-        <v>39.26</v>
+        <v>53.79</v>
       </c>
       <c r="H12">
-        <v>60.74</v>
+        <v>46.21</v>
       </c>
       <c r="I12">
-        <v>39.26</v>
+        <v>53.79</v>
       </c>
       <c r="J12">
         <v>30</v>
@@ -913,63 +3457,63 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13">
-        <v>30.2</v>
+        <v>7.78</v>
       </c>
       <c r="F13">
-        <v>12.59</v>
+        <v>38.520000000000003</v>
       </c>
       <c r="G13">
-        <v>57.2</v>
+        <v>53.7</v>
       </c>
       <c r="H13">
-        <v>42.8</v>
+        <v>46.3</v>
       </c>
       <c r="I13">
-        <v>57.2</v>
+        <v>53.7</v>
       </c>
       <c r="J13">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14">
-        <v>27.25</v>
+        <v>33.31</v>
       </c>
       <c r="F14">
-        <v>16.78</v>
+        <v>14.09</v>
       </c>
       <c r="G14">
-        <v>55.97</v>
+        <v>52.6</v>
       </c>
       <c r="H14">
-        <v>44.03</v>
+        <v>47.4</v>
       </c>
       <c r="I14">
-        <v>55.97</v>
+        <v>52.6</v>
       </c>
       <c r="J14">
         <v>30</v>
@@ -977,39 +3521,39 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15">
-        <v>21.01</v>
+        <v>10.53</v>
       </c>
       <c r="F15">
-        <v>25.2</v>
+        <v>37.1</v>
       </c>
       <c r="G15">
-        <v>53.79</v>
+        <v>52.37</v>
       </c>
       <c r="H15">
-        <v>46.21</v>
+        <v>47.63</v>
       </c>
       <c r="I15">
-        <v>53.79</v>
+        <v>52.37</v>
       </c>
       <c r="J15">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>55</v>
@@ -1021,19 +3565,19 @@
         <v>13</v>
       </c>
       <c r="E16">
-        <v>33.31</v>
+        <v>32.22</v>
       </c>
       <c r="F16">
-        <v>14.09</v>
+        <v>15.47</v>
       </c>
       <c r="G16">
-        <v>52.6</v>
+        <v>52.32</v>
       </c>
       <c r="H16">
-        <v>47.4</v>
+        <v>47.68</v>
       </c>
       <c r="I16">
-        <v>52.6</v>
+        <v>52.32</v>
       </c>
       <c r="J16">
         <v>30</v>
@@ -1041,255 +3585,255 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17">
-        <v>10.53</v>
+        <v>40.1</v>
       </c>
       <c r="F17">
-        <v>37.1</v>
+        <v>10.11</v>
       </c>
       <c r="G17">
-        <v>52.37</v>
+        <v>49.78</v>
       </c>
       <c r="H17">
-        <v>47.63</v>
+        <v>50.22</v>
       </c>
       <c r="I17">
-        <v>52.37</v>
+        <v>49.78</v>
       </c>
       <c r="J17">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="E18">
-        <v>15.48</v>
+        <v>42.96</v>
       </c>
       <c r="F18">
-        <v>25.96</v>
+        <v>11.73</v>
       </c>
       <c r="G18">
-        <v>58.56</v>
+        <v>45.3</v>
       </c>
       <c r="H18">
-        <v>41.44</v>
+        <v>54.7</v>
       </c>
       <c r="I18">
-        <v>58.56</v>
+        <v>45.3</v>
       </c>
       <c r="J18">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="E19">
-        <v>10.65</v>
+        <v>32.229999999999997</v>
       </c>
       <c r="F19">
-        <v>27.27</v>
+        <v>28.51</v>
       </c>
       <c r="G19">
-        <v>62.07</v>
+        <v>39.26</v>
       </c>
       <c r="H19">
-        <v>37.93</v>
+        <v>60.74</v>
       </c>
       <c r="I19">
-        <v>62.07</v>
+        <v>39.26</v>
       </c>
       <c r="J19">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E20">
-        <v>7.78</v>
+        <v>51.6</v>
       </c>
       <c r="F20">
-        <v>38.520000000000003</v>
+        <v>11.04</v>
       </c>
       <c r="G20">
-        <v>53.7</v>
+        <v>37.369999999999997</v>
       </c>
       <c r="H20">
-        <v>46.3</v>
+        <v>62.63</v>
       </c>
       <c r="I20">
-        <v>53.7</v>
+        <v>37.369999999999997</v>
       </c>
       <c r="J20">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="E21">
-        <v>21.66</v>
+        <v>54.11</v>
       </c>
       <c r="F21">
-        <v>21.76</v>
+        <v>11.18</v>
       </c>
       <c r="G21">
-        <v>56.59</v>
+        <v>34.71</v>
       </c>
       <c r="H21">
-        <v>43.41</v>
+        <v>65.290000000000006</v>
       </c>
       <c r="I21">
-        <v>56.59</v>
+        <v>34.71</v>
       </c>
       <c r="J21">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="E22">
-        <v>42.96</v>
+        <v>58</v>
       </c>
       <c r="F22">
-        <v>11.73</v>
+        <v>9.51</v>
       </c>
       <c r="G22">
-        <v>45.3</v>
+        <v>32.49</v>
       </c>
       <c r="H22">
-        <v>54.7</v>
+        <v>67.510000000000005</v>
       </c>
       <c r="I22">
-        <v>45.3</v>
+        <v>32.49</v>
       </c>
       <c r="J22">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="E23">
-        <v>32.22</v>
+        <v>50.31</v>
       </c>
       <c r="F23">
-        <v>15.47</v>
+        <v>17.45</v>
       </c>
       <c r="G23">
-        <v>52.32</v>
+        <v>32.229999999999997</v>
       </c>
       <c r="H23">
-        <v>47.68</v>
+        <v>67.77</v>
       </c>
       <c r="I23">
-        <v>52.32</v>
+        <v>32.229999999999997</v>
       </c>
       <c r="J23">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E24">
-        <v>22.6</v>
+        <v>60.45</v>
       </c>
       <c r="F24">
-        <v>16.62</v>
+        <v>10.99</v>
       </c>
       <c r="G24">
-        <v>60.78</v>
+        <v>28.55</v>
       </c>
       <c r="H24">
-        <v>39.22</v>
+        <v>71.45</v>
       </c>
       <c r="I24">
-        <v>60.78</v>
+        <v>28.55</v>
       </c>
       <c r="J24">
         <v>20</v>
@@ -1297,38 +3841,44 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25">
-        <v>6.88</v>
+        <v>59.17</v>
       </c>
       <c r="F25">
-        <v>37.33</v>
+        <v>13</v>
       </c>
       <c r="G25">
-        <v>55.8</v>
+        <v>27.83</v>
       </c>
       <c r="H25">
-        <v>44.2</v>
+        <v>72.17</v>
       </c>
       <c r="I25">
-        <v>55.8</v>
+        <v>27.83</v>
       </c>
       <c r="J25">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1">
+    <sortState ref="A2:J25">
+      <sortCondition ref="H1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>